<commit_message>
Completed Phase 2 (A7-A20) evidence added!
</commit_message>
<xml_diff>
--- a/omercanyenigun/evidence.xlsx
+++ b/omercanyenigun/evidence.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10107"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/omercanyenigun/Desktop/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBDC05A9-7076-0B45-8D1C-BCEFD07B9C02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="12380" tabRatio="500" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView windowWidth="28800" windowHeight="12375" tabRatio="500" firstSheet="6" activeTab="20"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -44,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="97">
   <si>
     <t>TeamName</t>
   </si>
@@ -103,6 +97,9 @@
     <t>ocy</t>
   </si>
   <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
     <t>NFTID</t>
   </si>
   <si>
@@ -148,6 +145,9 @@
     <t>BD0295BD981116FF95CA29DA607738880DD3F9FD4C13D3D84802C80182689960</t>
   </si>
   <si>
+    <t>stars1xwa0plhtfk03843pm2tw2gxy635g09z3z954plhcesye7wayvvps5fs3aw</t>
+  </si>
+  <si>
     <t>elgafar-1</t>
   </si>
   <si>
@@ -160,56 +160,189 @@
     <t>5413A020A0532381864449136CD3BB15268E5DEF1B2565FCC01CA15B83D0A88E</t>
   </si>
   <si>
-    <t>stars1xwa0plhtfk03843pm2tw2gxy635g09z3z954plhcesye7wayvvps5fs3aw</t>
-  </si>
-  <si>
     <t>7F14944771B83D29A664BECC0C8B024D95C9C8D2F4D0507C3235639C0CCC6662</t>
   </si>
   <si>
+    <t>ibc/59092B916CC764C0496CB2BCE79B78D6F87DBD60748142EBA3733BE25C747590</t>
+  </si>
+  <si>
     <t>uptick_7000-2</t>
   </si>
   <si>
     <t>A8D51E86D5E20BC6356C8D247916165160ECCC370DC1909381DFCC36B1F1548D</t>
   </si>
   <si>
-    <t>ibc/59092B916CC764C0496CB2BCE79B78D6F87DBD60748142EBA3733BE25C747590</t>
-  </si>
-  <si>
     <t>CE5D2F6461A60E986DC2AB6DB0BF2FB5BDAF85D9B5F79FD2F16C3891E1D03359</t>
   </si>
   <si>
     <t>3B703BB571132BA508565503018625A23F23998D6F5168338B5FB47A758033CB</t>
   </si>
   <si>
-    <t>ibc class on chain</t>
-  </si>
-  <si>
-    <t>nft id</t>
-  </si>
-  <si>
-    <t>tx hash on that chain</t>
-  </si>
-  <si>
-    <t>chain id</t>
-  </si>
-  <si>
-    <t>tx hash on that chain	chain id</t>
+    <t>ibc/A02B1968CECA98D50D3AE4898A961881490CF9081D0569639B8E0E650A6CD66E</t>
+  </si>
+  <si>
+    <t>ibc/33AA248FFE42BC5CEE96C694FFDB551E23D683FA0190D13843E40C1AE0D7D555</t>
+  </si>
+  <si>
+    <t>ibc/BB125490BF0E85A134599BE877C3DECDB80B5E570908035C3509772543F22D5E</t>
+  </si>
+  <si>
+    <t>ibc/316909B75D2F9CEF93092E7975D33EBC4B67D375D41CC4C31E591AAA3069F7E7</t>
+  </si>
+  <si>
+    <t>nft7</t>
+  </si>
+  <si>
+    <t>ibc/E6B585355B7BE0BFFE95F2D2EB03A2B998FE027443B8E40981071A3E26A8BC91</t>
+  </si>
+  <si>
+    <t>nft8</t>
+  </si>
+  <si>
+    <t>ibc/1D1F943597DF85F1EAC69B4BB369C3F87B756F3015C73D334C30D8F827717118</t>
+  </si>
+  <si>
+    <t>nft9</t>
+  </si>
+  <si>
+    <t>7B99FCFCB4B19875B897C172C9C8C9EFF41B7E4268784D1092213573670E9FE2</t>
+  </si>
+  <si>
+    <t>gon-irishub-1</t>
+  </si>
+  <si>
+    <t>61BE74F0A450EBC0ECBFCDDE266D7DD294BC72F31F56F040D8AFC51DDB96BB74</t>
+  </si>
+  <si>
+    <t>253EF8164187D81AF916FEF22E052A032340B748C4AF0813EF36E8D7D05E7B91</t>
+  </si>
+  <si>
+    <t>83A6844DDFC13AC82EBE878B13873C7AE18AA30E00FE354452F326F5C6AEE797</t>
+  </si>
+  <si>
+    <t>799D235D2CE692DF22BC66638532E89F95C1D25315A2AEA8CF36F8ECCCC386CA</t>
+  </si>
+  <si>
+    <t>2FF22BAF491A7F9E5121520260C1B3AB4D254F218BC09B348374A6E2A266EF44</t>
+  </si>
+  <si>
+    <t>8EE4CEF0381BDAA1E38988C1A58C691101076BA3F991446624C1A8998BCC33B7</t>
+  </si>
+  <si>
+    <t>gon-flixnet-1</t>
+  </si>
+  <si>
+    <t>A811BFFE6F75A23FDC135219CD9ECC0A6FA6A48A5F380CC25CD3C92B025E01C0</t>
+  </si>
+  <si>
+    <t>704D4B81859338BBEDC3C9832DDDF8C1BBB3C55A2C332E97C102FCDC63705A63</t>
+  </si>
+  <si>
+    <t>21DF65F0C9262774141EC5D4126DD822931FBFD1FE439496B5481AE401DE7044</t>
+  </si>
+  <si>
+    <t>uni-6</t>
+  </si>
+  <si>
+    <t>3EFADE1FE3881BF368DB69256CAF5ABB7FBA8BB4FD2C95A2445C452CDFD49D55</t>
+  </si>
+  <si>
+    <t>7D1937AD855630A42E55A9F321C88BD83858011887D033B94900A3A5394CEF04</t>
+  </si>
+  <si>
+    <t>CE2FD23E692AF39860E969B8F5737CA7D4E16B80CD91751056D521B0ADD3B548</t>
+  </si>
+  <si>
+    <t>E4C2EE5DE991679BF11EAA6235AB2555CA57158F3410621C0446672BDA1F8FF3</t>
+  </si>
+  <si>
+    <t>B7FFB3C9C04939E78B9AE4E918A700023E21A3EF9AAA4BED824EAC280B69E011</t>
+  </si>
+  <si>
+    <t>B5DC2789B37C8CFFC34D127404D5D201B884FE430C853C2D2E3E40E6033A9DEB</t>
+  </si>
+  <si>
+    <t>A87376AFFC8FF55C22F9B169BD8BD9E6DF2F4015B26BAA71C281BEA9DAF2FA77</t>
+  </si>
+  <si>
+    <t>00A6A4C7BC615950356522C2E0A245FCD73B15284F4288EC221675058DA339E7</t>
+  </si>
+  <si>
+    <t>8335680ACD7A26E3513717D3A06310DCD48D413EEA21FA04577CDA76B3ECF98B</t>
+  </si>
+  <si>
+    <t>44C84CAF74F6CAA0CCDCF298A8FAB27F7210F9D3D2FF52F473F2EA939DA72D48</t>
+  </si>
+  <si>
+    <t>DD84C4A9F1FF22414B68DF28891BDA2E6DEFA042499B1F749D6F7AC503231638</t>
+  </si>
+  <si>
+    <t>24875CFC6557F5E1985EB7A2D0ADCB10A187D5A4961A0A60F098A6FA201FAADC</t>
+  </si>
+  <si>
+    <t>97AA9A3DC36DD7FB244BC7E211CED89F6FEFBF667A841B1997DDC607AAE55624</t>
+  </si>
+  <si>
+    <t>EC0809458F2CB619B1DC5E44F240B30321A3B93A068663018B7B2BF03FF1D742</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gon-flixnet-1
+</t>
+  </si>
+  <si>
+    <t>5E9D82615E0FA0F1E287624FA742CCAD52ECC189B7D315FA9E6B80083E8D7EF7</t>
+  </si>
+  <si>
+    <t>CD6292A4A2C3E3D28ECBF3F5234561FF9C7F2513894C8FEBA3FAEFFBF50419FF</t>
+  </si>
+  <si>
+    <t>20C4F32FE10B0F9632202149D97BBC5A4E70A6151F2F8048650696A6F08E0AC4</t>
+  </si>
+  <si>
+    <t>98CD7F653B2641C5C2A66AD9B7F0EF9FB9E89284EB021FB65895D494650B5899</t>
+  </si>
+  <si>
+    <t>51438E5C659F7A74D06DBE6AA8E4BE43D4673C6E579B1E81534582BBE06635D9</t>
+  </si>
+  <si>
+    <t>5C24F898CACB29BFDCE7F9FC8189C9C0489C306D6FBDFE480B972FFC38EFA21C</t>
+  </si>
+  <si>
+    <t>38D7DCACEA7FB75E4954FA55352D791A239D1E30B4ECAD729D32C068E5E9549A</t>
+  </si>
+  <si>
+    <t>E2A6D623D4762B00B851344D9190DCA70EB5B5214751AFF9845BE0900745C62D</t>
+  </si>
+  <si>
+    <t>073D8351FBF97D4BFFBD72AC6CAC6434B1777C2401EB7740A9A687D0C9553E51</t>
+  </si>
+  <si>
+    <t>8A3D18E25BA7C276E61CED23B65662563EF36AD9E4B9E85948A47A26E71FBB11</t>
+  </si>
+  <si>
+    <t>749E7D4186EF947D54E308586C4F297EC9AF9ABBAAC4E9B3BE0676FB4A7B2C2E</t>
+  </si>
+  <si>
+    <t>31FDB9C27136AA7BBCDE279FF05E82516DE89A4253A64FF8EF21513F1E68EC33</t>
   </si>
   <si>
     <t>The first Interchain NFT-Transfer TxHash</t>
   </si>
   <si>
     <t>The Internal Transfer TxHash on IRISnet</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="24">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -234,8 +367,159 @@
       <name val="Calibri"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -248,8 +532,194 @@
         <bgColor rgb="FFC0C0C0"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -257,22 +727,267 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="23" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="23" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -280,10 +995,57 @@
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
+    <cellStyle name="Comma" xfId="2" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
+    <cellStyle name="Currency" xfId="5" builtinId="4"/>
+    <cellStyle name="Percent" xfId="6" builtinId="5"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8"/>
+    <cellStyle name="60% - Accent4" xfId="8" builtinId="44"/>
+    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9"/>
+    <cellStyle name="Check Cell" xfId="10" builtinId="23"/>
+    <cellStyle name="Heading 2" xfId="11" builtinId="17"/>
+    <cellStyle name="Note" xfId="12" builtinId="10"/>
+    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
+    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
+    <cellStyle name="Title" xfId="16" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
+    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
+    <cellStyle name="Input" xfId="21" builtinId="20"/>
+    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
+    <cellStyle name="Good" xfId="23" builtinId="26"/>
+    <cellStyle name="Output" xfId="24" builtinId="21"/>
+    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
+    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
+    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
+    <cellStyle name="Total" xfId="28" builtinId="25"/>
+    <cellStyle name="Bad" xfId="29" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
+    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
+    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
+    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
+    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
+    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
+    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
+    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
@@ -356,9 +1118,6 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -616,30 +1375,30 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B2" sqref="B2:F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="12.6666666666667" defaultRowHeight="12.75" outlineLevelRow="2" outlineLevelCol="7"/>
   <cols>
-    <col min="1" max="1" width="14.6640625" customWidth="1"/>
-    <col min="2" max="2" width="14.83203125" customWidth="1"/>
-    <col min="3" max="3" width="17.5" customWidth="1"/>
-    <col min="4" max="4" width="16.1640625" customWidth="1"/>
-    <col min="5" max="5" width="18.1640625" customWidth="1"/>
-    <col min="6" max="6" width="17.6640625" customWidth="1"/>
-    <col min="7" max="7" width="14.6640625" customWidth="1"/>
+    <col min="1" max="1" width="14.6666666666667" customWidth="1"/>
+    <col min="2" max="2" width="14.8285714285714" customWidth="1"/>
+    <col min="3" max="3" width="17.5047619047619" customWidth="1"/>
+    <col min="4" max="4" width="16.1619047619048" customWidth="1"/>
+    <col min="5" max="5" width="18.1619047619048" customWidth="1"/>
+    <col min="6" max="6" width="17.6666666666667" customWidth="1"/>
+    <col min="7" max="7" width="14.6666666666667" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="14" x14ac:dyDescent="0.15">
+    <row r="1" ht="14.25" spans="1:8">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -665,11 +1424,11 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="14" x14ac:dyDescent="0.15">
-      <c r="A2" s="8" t="s">
+    <row r="2" ht="14.25" spans="1:8">
+      <c r="A2" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="9" t="s">
         <v>9</v>
       </c>
       <c r="C2" s="3" t="s">
@@ -689,420 +1448,546 @@
       </c>
       <c r="H2" s="3"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A3" s="8"/>
-      <c r="B3" s="8"/>
+    <row r="3" spans="1:2">
+      <c r="A3" s="9"/>
+      <c r="B3" s="9"/>
     </row>
   </sheetData>
-  <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="12.6666666666667" defaultRowHeight="12.75" outlineLevelRow="1" outlineLevelCol="1"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="14" x14ac:dyDescent="0.15">
+    <row r="1" ht="14.25" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="14" x14ac:dyDescent="0.15">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" ht="14.25" spans="1:2">
       <c r="A2" s="3" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="12.6666666666667" defaultRowHeight="12.75" outlineLevelRow="1" outlineLevelCol="1"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="14" x14ac:dyDescent="0.15">
+    <row r="1" ht="14.25" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="14" x14ac:dyDescent="0.15">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" ht="14.25" spans="1:2">
       <c r="A2" s="3" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="12.6666666666667" defaultRowHeight="12.75" outlineLevelRow="1" outlineLevelCol="1"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="14" x14ac:dyDescent="0.15">
+    <row r="1" ht="14.25" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="14" x14ac:dyDescent="0.15">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" ht="14.25" spans="1:2">
       <c r="A2" s="3" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="12.6666666666667" defaultRowHeight="12.75" outlineLevelRow="1" outlineLevelCol="1"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="14" x14ac:dyDescent="0.15">
+    <row r="1" ht="14.25" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="14" x14ac:dyDescent="0.15">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" ht="14.25" spans="1:2">
       <c r="A2" s="3" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
-  <dimension ref="A1:B4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="12.6666666666667" defaultRowHeight="12.75" outlineLevelRow="4" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="1" width="31.5" customWidth="1"/>
+    <col min="1" max="1" width="31.5047619047619" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="14" x14ac:dyDescent="0.15">
+    <row r="1" ht="14.25" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="14" x14ac:dyDescent="0.15">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" ht="14.25" spans="1:2">
       <c r="A2" s="3" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="14" x14ac:dyDescent="0.15">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" ht="14.25" spans="1:2">
       <c r="A3" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="14" x14ac:dyDescent="0.15">
+        <v>57</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" ht="14.25" spans="1:2">
       <c r="A4" s="3" t="s">
-        <v>49</v>
+        <v>58</v>
+      </c>
+      <c r="B4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" ht="14.25" spans="1:2">
+      <c r="A5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
-  <dimension ref="A1:B4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="12.6666666666667" defaultRowHeight="12.75" outlineLevelRow="4" outlineLevelCol="1"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="14" x14ac:dyDescent="0.15">
+    <row r="1" ht="14.25" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="14" x14ac:dyDescent="0.15">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" ht="14.25" spans="1:2">
       <c r="A2" s="3" t="s">
-        <v>47</v>
+        <v>60</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="14" x14ac:dyDescent="0.15">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" ht="14.25" spans="1:2">
       <c r="A3" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="14" x14ac:dyDescent="0.15">
+        <v>61</v>
+      </c>
+      <c r="B3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" ht="14.25" spans="1:2">
       <c r="A4" s="3" t="s">
-        <v>49</v>
+        <v>62</v>
+      </c>
+      <c r="B4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B5" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
-  <dimension ref="A1:B4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="12.6666666666667" defaultRowHeight="12.75" outlineLevelRow="4" outlineLevelCol="1"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="14" x14ac:dyDescent="0.15">
+    <row r="1" ht="14.25" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="14" x14ac:dyDescent="0.15">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" ht="14.25" spans="1:2">
       <c r="A2" s="3" t="s">
-        <v>47</v>
+        <v>65</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="14" x14ac:dyDescent="0.15">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" ht="14.25" spans="1:2">
       <c r="A3" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="14" x14ac:dyDescent="0.15">
+        <v>66</v>
+      </c>
+      <c r="B3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="4" ht="14.25" spans="1:2">
       <c r="A4" s="3" t="s">
-        <v>49</v>
+        <v>68</v>
+      </c>
+      <c r="B4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>69</v>
+      </c>
+      <c r="B5" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
-  <dimension ref="A1:B4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="12.6666666666667" defaultRowHeight="12.75" outlineLevelRow="4" outlineLevelCol="1"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="14" x14ac:dyDescent="0.15">
+    <row r="1" ht="14.25" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="14" x14ac:dyDescent="0.15">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" ht="14.25" spans="1:2">
       <c r="A2" s="3" t="s">
-        <v>47</v>
+        <v>70</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="14" x14ac:dyDescent="0.15">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" ht="14.25" spans="1:2">
       <c r="A3" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="14" x14ac:dyDescent="0.15">
+        <v>71</v>
+      </c>
+      <c r="B3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="4" ht="14.25" spans="1:2">
       <c r="A4" s="3" t="s">
-        <v>49</v>
+        <v>72</v>
+      </c>
+      <c r="B4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>73</v>
+      </c>
+      <c r="B5" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
-  <dimension ref="A1:B4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H34" sqref="H34"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="12.6666666666667" defaultRowHeight="12.75" outlineLevelRow="4" outlineLevelCol="1"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="14" x14ac:dyDescent="0.15">
+    <row r="1" ht="14.25" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="14" x14ac:dyDescent="0.15">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" ht="14.25" spans="1:2">
       <c r="A2" s="3" t="s">
-        <v>47</v>
+        <v>74</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="14" x14ac:dyDescent="0.15">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" ht="14.25" spans="1:2">
       <c r="A3" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="14" x14ac:dyDescent="0.15">
+        <v>75</v>
+      </c>
+      <c r="B3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" ht="14.25" spans="1:2">
       <c r="A4" s="3" t="s">
-        <v>49</v>
+        <v>76</v>
+      </c>
+      <c r="B4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>77</v>
+      </c>
+      <c r="B5" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
-  <dimension ref="A1:B4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="12.6666666666667" defaultRowHeight="12.75" outlineLevelRow="4" outlineLevelCol="1"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="14" x14ac:dyDescent="0.15">
+    <row r="1" ht="14.25" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="14" x14ac:dyDescent="0.15">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" ht="14.25" spans="1:2">
       <c r="A2" s="3" t="s">
-        <v>47</v>
+        <v>78</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="14" x14ac:dyDescent="0.15">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" ht="14.25" spans="1:2">
       <c r="A3" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="14" x14ac:dyDescent="0.15">
+        <v>79</v>
+      </c>
+      <c r="B3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="4" ht="14.25" spans="1:2">
       <c r="A4" s="3" t="s">
-        <v>49</v>
+        <v>80</v>
+      </c>
+      <c r="B4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" ht="25.5" spans="1:2">
+      <c r="A5" t="s">
+        <v>81</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>82</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="12.6666666666667" defaultRowHeight="12.75" outlineLevelCol="2"/>
   <cols>
-    <col min="1" max="2" width="17.83203125" customWidth="1"/>
+    <col min="1" max="2" width="17.8285714285714" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+    <row r="1" ht="14.25" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
@@ -1110,7 +1995,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+    <row r="2" ht="14.25" spans="1:2">
       <c r="A2" s="3" t="s">
         <v>17</v>
       </c>
@@ -1118,129 +2003,201 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="14" spans="3:3">
       <c r="C14" t="s">
-        <v>52</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
-  <dimension ref="A1:B4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="12.6666666666667" defaultRowHeight="12.75" outlineLevelRow="6" outlineLevelCol="1"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="14" x14ac:dyDescent="0.15">
+    <row r="1" ht="14.25" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="14" x14ac:dyDescent="0.15">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" ht="14.25" spans="1:2">
       <c r="A2" s="3" t="s">
-        <v>47</v>
+        <v>83</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="14" x14ac:dyDescent="0.15">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" ht="14.25" spans="1:2">
       <c r="A3" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="14" x14ac:dyDescent="0.15">
+        <v>84</v>
+      </c>
+      <c r="B3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" ht="14.25" spans="1:2">
       <c r="A4" s="3" t="s">
-        <v>49</v>
+        <v>85</v>
+      </c>
+      <c r="B4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>86</v>
+      </c>
+      <c r="B5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>87</v>
+      </c>
+      <c r="B6" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>88</v>
+      </c>
+      <c r="B7" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
-  <dimension ref="A1:B4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="12.6666666666667" defaultRowHeight="12.75" outlineLevelRow="6" outlineLevelCol="1"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="14" x14ac:dyDescent="0.15">
+    <row r="1" ht="14.25" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="14" x14ac:dyDescent="0.15">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" ht="14.25" spans="1:2">
       <c r="A2" s="3" t="s">
-        <v>47</v>
+        <v>89</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="14" x14ac:dyDescent="0.15">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" ht="14.25" spans="1:2">
       <c r="A3" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="14" x14ac:dyDescent="0.15">
+        <v>90</v>
+      </c>
+      <c r="B3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" ht="14.25" spans="1:2">
       <c r="A4" s="3" t="s">
-        <v>49</v>
+        <v>91</v>
+      </c>
+      <c r="B4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>92</v>
+      </c>
+      <c r="B5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>93</v>
+      </c>
+      <c r="B6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>94</v>
+      </c>
+      <c r="B7" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11.5047619047619" defaultRowHeight="12.75" outlineLevelRow="2"/>
   <sheetData>
-    <row r="1" spans="1:1" ht="14" x14ac:dyDescent="0.15">
+    <row r="1" ht="14.25" spans="1:1">
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" ht="16.5" customHeight="1" spans="1:1">
       <c r="A2" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" ht="14" x14ac:dyDescent="0.15">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="3" ht="14.25" spans="1:1">
       <c r="A3" s="3" t="s">
-        <v>51</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
@@ -1249,33 +2206,34 @@
 </file>
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11.5047619047619" defaultRowHeight="12.75" outlineLevelRow="2"/>
   <sheetData>
-    <row r="1" spans="1:1" ht="14" x14ac:dyDescent="0.15">
+    <row r="1" ht="14.25" spans="1:1">
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="14" x14ac:dyDescent="0.15">
+    <row r="2" ht="14.25" spans="1:1">
       <c r="A2" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" ht="14" x14ac:dyDescent="0.15">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="3" ht="14.25" spans="1:1">
       <c r="A3" s="3" t="s">
-        <v>51</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
@@ -1284,33 +2242,34 @@
 </file>
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11.5047619047619" defaultRowHeight="12.75" outlineLevelRow="2"/>
   <sheetData>
-    <row r="1" spans="1:1" ht="14" x14ac:dyDescent="0.15">
+    <row r="1" ht="14.25" spans="1:1">
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="14" x14ac:dyDescent="0.15">
+    <row r="2" ht="14.25" spans="1:1">
       <c r="A2" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" ht="14" x14ac:dyDescent="0.15">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="3" ht="14.25" spans="1:1">
       <c r="A3" s="3" t="s">
-        <v>51</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
@@ -1319,33 +2278,34 @@
 </file>
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11.5047619047619" defaultRowHeight="12.75" outlineLevelRow="2"/>
   <sheetData>
-    <row r="1" spans="1:1" ht="14" x14ac:dyDescent="0.15">
+    <row r="1" ht="14.25" spans="1:1">
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="14" x14ac:dyDescent="0.15">
+    <row r="2" ht="14.25" spans="1:1">
       <c r="A2" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" ht="14" x14ac:dyDescent="0.15">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="3" ht="14.25" spans="1:1">
       <c r="A3" s="3" t="s">
-        <v>51</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
@@ -1354,20 +2314,21 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="12.6666666666667" defaultRowHeight="12.75" outlineLevelRow="6" outlineLevelCol="2"/>
   <cols>
-    <col min="1" max="2" width="17.83203125" customWidth="1"/>
+    <col min="1" max="2" width="17.8285714285714" customWidth="1"/>
     <col min="3" max="3" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+    <row r="1" ht="14.25" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
@@ -1375,98 +2336,100 @@
         <v>16</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" ht="14.25" spans="1:3">
       <c r="A2" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>18</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" ht="14.25" spans="1:3">
       <c r="A3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>18</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" ht="14.25" spans="1:3">
       <c r="A4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>18</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" ht="14.25" spans="1:3">
       <c r="A5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>18</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" ht="14.25" spans="1:3">
       <c r="A6" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>18</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" ht="14.25" spans="1:3">
       <c r="A7" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>18</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="12.6666666666667" defaultRowHeight="12.75" outlineLevelCol="5"/>
   <cols>
-    <col min="1" max="2" width="17.83203125" customWidth="1"/>
+    <col min="1" max="2" width="17.8285714285714" customWidth="1"/>
     <col min="3" max="3" width="16" customWidth="1"/>
-    <col min="4" max="4" width="13.6640625" customWidth="1"/>
+    <col min="4" max="4" width="13.6666666666667" customWidth="1"/>
     <col min="5" max="5" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="14" x14ac:dyDescent="0.15">
+    <row r="1" ht="14.25" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
@@ -1474,103 +2437,105 @@
         <v>16</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" ht="14.25" spans="1:4">
       <c r="A2" s="3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" ht="14.25" spans="1:4">
+      <c r="A3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" ht="15" customHeight="1" spans="1:6">
+      <c r="A4" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="15" x14ac:dyDescent="0.15">
-      <c r="A3" t="s">
+      <c r="B4" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="C3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
+      <c r="C4" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="E4" s="5"/>
+      <c r="E4" s="7"/>
       <c r="F4" s="2"/>
     </row>
-    <row r="5" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" ht="12" customHeight="1" spans="1:6">
       <c r="A5" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
     </row>
-    <row r="8" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="E8" s="5"/>
+    <row r="8" ht="15" spans="5:6">
+      <c r="E8" s="7"/>
       <c r="F8" s="2"/>
     </row>
-    <row r="9" spans="1:6" ht="14" x14ac:dyDescent="0.15">
+    <row r="9" ht="14.25" spans="5:6">
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
     </row>
   </sheetData>
-  <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="12.6666666666667" defaultRowHeight="12.75" outlineLevelCol="5"/>
   <cols>
-    <col min="1" max="2" width="17.83203125" customWidth="1"/>
+    <col min="1" max="2" width="17.8285714285714" customWidth="1"/>
     <col min="3" max="3" width="16" customWidth="1"/>
     <col min="4" max="4" width="18" customWidth="1"/>
-    <col min="5" max="5" width="47.5" customWidth="1"/>
+    <col min="5" max="5" width="47.5047619047619" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="14" x14ac:dyDescent="0.15">
+    <row r="1" ht="14.25" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
@@ -1578,81 +2543,83 @@
         <v>16</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" ht="16" customHeight="1" spans="1:4">
+      <c r="A2" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" ht="14.25" spans="1:4">
+      <c r="A3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="B2" s="4" t="s">
+      <c r="D3" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="15" x14ac:dyDescent="0.15">
-      <c r="A3" t="s">
-        <v>41</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="E4" s="7"/>
-    </row>
-    <row r="5" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="E5" s="5"/>
+    </row>
+    <row r="4" ht="12" customHeight="1" spans="5:5">
+      <c r="E4" s="8"/>
+    </row>
+    <row r="5" ht="15" spans="5:6">
+      <c r="E5" s="7"/>
       <c r="F5" s="2"/>
     </row>
-    <row r="6" spans="1:6" ht="14" x14ac:dyDescent="0.15">
+    <row r="6" ht="14.25" spans="5:6">
       <c r="E6" s="3"/>
-      <c r="F6" s="4"/>
-    </row>
-    <row r="8" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="E8" s="5"/>
+      <c r="F6" s="5"/>
+    </row>
+    <row r="8" ht="15" spans="5:6">
+      <c r="E8" s="7"/>
       <c r="F8" s="2"/>
     </row>
-    <row r="9" spans="1:6" ht="14" x14ac:dyDescent="0.15">
+    <row r="9" ht="14.25" spans="5:5">
       <c r="E9" s="3"/>
     </row>
   </sheetData>
-  <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E6" sqref="E6:F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="12.6666666666667" defaultRowHeight="12.75" outlineLevelRow="6" outlineLevelCol="5"/>
   <cols>
-    <col min="1" max="2" width="17.83203125" customWidth="1"/>
+    <col min="1" max="2" width="17.8285714285714" customWidth="1"/>
     <col min="3" max="3" width="16" customWidth="1"/>
-    <col min="4" max="4" width="17.1640625" customWidth="1"/>
-    <col min="5" max="5" width="18.5" customWidth="1"/>
+    <col min="4" max="4" width="17.1619047619048" customWidth="1"/>
+    <col min="5" max="5" width="18.5047619047619" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="14" x14ac:dyDescent="0.15">
+    <row r="1" ht="14.25" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
@@ -1660,57 +2627,59 @@
         <v>16</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.15">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" ht="13" customHeight="1" spans="1:4">
       <c r="A2" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="E6" s="5"/>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" ht="15" spans="5:6">
+      <c r="E6" s="7"/>
       <c r="F6" s="2"/>
     </row>
-    <row r="7" spans="1:6" ht="14" x14ac:dyDescent="0.15">
+    <row r="7" ht="14.25" spans="5:6">
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
     </row>
   </sheetData>
-  <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="12.6666666666667" defaultRowHeight="12.75" outlineLevelRow="6" outlineLevelCol="5"/>
   <cols>
-    <col min="1" max="1" width="17.83203125" customWidth="1"/>
+    <col min="1" max="1" width="17.8285714285714" customWidth="1"/>
     <col min="2" max="2" width="16" customWidth="1"/>
-    <col min="3" max="3" width="16.33203125" customWidth="1"/>
-    <col min="4" max="4" width="14.33203125" customWidth="1"/>
+    <col min="3" max="3" width="16.3333333333333" customWidth="1"/>
+    <col min="4" max="4" width="14.3333333333333" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="14" x14ac:dyDescent="0.15">
+    <row r="1" ht="14.25" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
@@ -1718,102 +2687,111 @@
         <v>16</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" ht="14.25" spans="1:4">
       <c r="A2" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="B2" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="E6" s="5"/>
+    </row>
+    <row r="6" ht="15" spans="5:6">
+      <c r="E6" s="7"/>
       <c r="F6" s="2"/>
     </row>
-    <row r="7" spans="1:6" ht="14" x14ac:dyDescent="0.15">
+    <row r="7" ht="14.25" spans="5:6">
       <c r="E7" s="3"/>
-      <c r="F7" s="4"/>
+      <c r="F7" s="5"/>
     </row>
   </sheetData>
-  <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="12.6666666666667" defaultRowHeight="12.75" outlineLevelRow="1" outlineLevelCol="1"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="14" x14ac:dyDescent="0.15">
+    <row r="1" ht="14.25" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="14" x14ac:dyDescent="0.15">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" ht="14.25" spans="1:2">
       <c r="A2" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>46</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="12.6666666666667" defaultRowHeight="12.75" outlineLevelRow="1" outlineLevelCol="1"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="14" x14ac:dyDescent="0.15">
+    <row r="1" ht="14.25" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="14" x14ac:dyDescent="0.15">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" ht="14.25" spans="1:2">
       <c r="A2" s="3" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>46</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>